<commit_message>
Updates to final project from in-class working session
</commit_message>
<xml_diff>
--- a/final project/question_brainstorm.xlsx
+++ b/final project/question_brainstorm.xlsx
@@ -499,7 +499,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Work from class 18 and worked in final project
For final project - formatted candidates reveal section
</commit_message>
<xml_diff>
--- a/final project/question_brainstorm.xlsx
+++ b/final project/question_brainstorm.xlsx
@@ -28,12 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>TV Show</t>
-  </si>
-  <si>
-    <t>Hillary Clinton</t>
   </si>
   <si>
     <t>Parks &amp; Rec</t>
@@ -176,6 +173,30 @@
   </si>
   <si>
     <t>Everything in life is luck.</t>
+  </si>
+  <si>
+    <t>Hillary</t>
+  </si>
+  <si>
+    <t>blackberry</t>
+  </si>
+  <si>
+    <t>lindsay graham</t>
+  </si>
+  <si>
+    <t>iphone</t>
+  </si>
+  <si>
+    <t>Favorite Tech Device</t>
+  </si>
+  <si>
+    <t>favorite drinks</t>
+  </si>
+  <si>
+    <t>wine</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -496,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,179 +533,204 @@
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on Q1 and Q5
</commit_message>
<xml_diff>
--- a/final project/question_brainstorm.xlsx
+++ b/final project/question_brainstorm.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
   <si>
     <t>TV Show</t>
   </si>
@@ -187,9 +187,6 @@
     <t>iphone</t>
   </si>
   <si>
-    <t>Favorite Tech Device</t>
-  </si>
-  <si>
     <t>favorite drinks</t>
   </si>
   <si>
@@ -197,6 +194,48 @@
   </si>
   <si>
     <t>water</t>
+  </si>
+  <si>
+    <t>By blaming others, we fail to find the real solution to our problems and we do not carry out our own responsibilities.</t>
+  </si>
+  <si>
+    <t>Favorite tech device</t>
+  </si>
+  <si>
+    <t>plane</t>
+  </si>
+  <si>
+    <t>College Major</t>
+  </si>
+  <si>
+    <t>political science</t>
+  </si>
+  <si>
+    <t>law</t>
+  </si>
+  <si>
+    <t>Hamburgers</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Favorite book</t>
+  </si>
+  <si>
+    <t>Fyodor Dostoyevsky's "The Brothers Karamazov"</t>
+  </si>
+  <si>
+    <t>Art of the Deal or Bible</t>
+  </si>
+  <si>
+    <t>By the people: Rebuilding Liberty Without Permission.</t>
+  </si>
+  <si>
+    <t>Nobody can hinder you from doing what you want, if that’s what you set your mind to.</t>
   </si>
 </sst>
 </file>
@@ -212,12 +251,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -232,11 +277,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,33 +563,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.5703125" customWidth="1"/>
+    <col min="2" max="5" width="25.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
@@ -566,13 +610,13 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -585,16 +629,16 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
@@ -614,123 +658,168 @@
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E13" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>37</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="G20" t="s">
         <v>54</v>
-      </c>
-      <c r="G18" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>